<commit_message>
Fix first name/lastname display bug
</commit_message>
<xml_diff>
--- a/docs/test_data_2 - Copy.xlsx
+++ b/docs/test_data_2 - Copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LG4000\Desktop\comms\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985A2E2D-CBBB-451D-872E-8D65C5BBA98E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F45BCA-EEDE-4F10-87B5-AEB813162ED3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B3B8992A-2509-491A-9C39-2580EA4D3B1D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>Count</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>MANILA</t>
-  </si>
-  <si>
-    <t>Chong</t>
   </si>
   <si>
     <t>Nicholas</t>
@@ -657,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CEAC2C5-08A0-40A6-93E9-BE2759C1F504}">
   <dimension ref="A1:Y147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="121" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="121" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -756,11 +753,9 @@
       <c r="D2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
@@ -827,9 +822,7 @@
       <c r="D3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>36</v>
       </c>
@@ -900,9 +893,7 @@
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>